<commit_message>
[FIX] iCC644 LDH-D enzyme [ADD] escher maps
</commit_message>
<xml_diff>
--- a/results/results_topological_analysis.xlsx
+++ b/results/results_topological_analysis.xlsx
@@ -1,32 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView activeTab="2" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="12576" windowWidth="23256" xWindow="-108" yWindow="-108"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="iCC390" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="iCC431" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="iCC464" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="iCC644" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="iCC390" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="iCC431" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="iCC464" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="iCC644" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <b val="1"/>
+      <sz val="11"/>
     </font>
     <font>
       <b val="1"/>
@@ -40,12 +45,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -57,18 +77,21 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+  <cellXfs count="3">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf applyAlignment="1" borderId="2" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -432,10 +455,15 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="B2" sqref="B2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <cols>
+    <col bestFit="1" customWidth="1" max="2" min="2" width="10.109375"/>
+    <col bestFit="1" customWidth="1" max="3" min="3" width="10"/>
+    <col bestFit="1" customWidth="1" max="6" min="6" width="17.33203125"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
@@ -503,7 +531,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
@@ -516,10 +544,14 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="E2" sqref="D2:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <cols>
+    <col bestFit="1" customWidth="1" max="2" min="2" width="10.109375"/>
+    <col bestFit="1" customWidth="1" max="3" min="3" width="10"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
@@ -587,7 +619,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
@@ -599,11 +631,11 @@
   </sheetPr>
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
@@ -671,7 +703,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
@@ -690,44 +722,44 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>e reactions</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>c reactions</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" s="2" t="inlineStr">
         <is>
           <t>e metabolites</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" s="2" t="inlineStr">
         <is>
           <t>c metabolites</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" s="2" t="inlineStr">
         <is>
           <t>exchange reactions</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="G1" s="2" t="inlineStr">
         <is>
           <t>genes</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="H1" s="2" t="inlineStr">
         <is>
           <t>GPRs</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="inlineStr">
+      <c r="A2" s="2" t="inlineStr">
         <is>
           <t>total</t>
         </is>
@@ -736,7 +768,7 @@
         <v>267</v>
       </c>
       <c r="C2" t="n">
-        <v>737</v>
+        <v>738</v>
       </c>
       <c r="D2" t="n">
         <v>135</v>
@@ -748,13 +780,13 @@
         <v>136</v>
       </c>
       <c r="G2" t="n">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="H2" t="n">
-        <v>679</v>
+        <v>680</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>